<commit_message>
Updated results with ned RNG
</commit_message>
<xml_diff>
--- a/Project3/brute_data_6.xlsx
+++ b/Project3/brute_data_6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\Documents\ComputationalPhysics\Projects\Gruppe\Project3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tore/Documents/2019 høst/Computational-Physics-group/Project3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BA70D5-7EB3-4347-8EF5-00662B76E0F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E9819B3-0E85-3E45-AF43-9D17DD8F9CD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="560" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="brute_data_6" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,29 +35,29 @@
     <t>STD</t>
   </si>
   <si>
-    <t>INTEGRAL</t>
+    <t>Integral</t>
   </si>
   <si>
-    <t>TIME</t>
+    <t>Time</t>
   </si>
   <si>
-    <t>AVG</t>
+    <t>Avg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -93,28 +95,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -122,7 +124,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -130,14 +132,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -145,14 +147,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -160,7 +162,7 @@
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -168,14 +170,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -879,20 +881,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.06640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -903,151 +901,151 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2">
-        <v>2.3369500000000001E-2</v>
+        <v>1.9327199999999999E-2</v>
       </c>
       <c r="C2">
-        <v>0.20399485789999999</v>
+        <v>0.1962515702</v>
       </c>
       <c r="D2">
-        <v>6.4447000000000004E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.113072359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>2.2042093759999999E-2</v>
+        <v>1.783849425E-2</v>
       </c>
       <c r="C3">
-        <v>0.1930129079</v>
+        <v>0.1821007526</v>
       </c>
       <c r="D3">
-        <v>6.2504299999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <v>9.8292862999999994E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>1.3115736019999999E-2</v>
+        <v>1.276449707E-2</v>
       </c>
       <c r="C4">
-        <v>0.15723827509999999</v>
+        <v>0.14638135290000001</v>
       </c>
       <c r="D4">
-        <v>6.2660099999999996E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+        <v>7.1126959000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>1.2518355809999999E-2</v>
+        <v>5.3309816060000001E-2</v>
       </c>
       <c r="C5">
-        <v>0.14801033490000001</v>
+        <v>0.24086790890000001</v>
       </c>
       <c r="D5">
-        <v>6.3649600000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.107232693</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>1.8605360479999999E-2</v>
+        <v>0.20664666340000001</v>
       </c>
       <c r="C6">
-        <v>0.1870214707</v>
+        <v>0.37170256460000001</v>
       </c>
       <c r="D6">
-        <v>7.1078500000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.103188738</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>1.960357578E-2</v>
+        <v>8.0532306070000004E-2</v>
       </c>
       <c r="C7">
-        <v>0.1579829096</v>
+        <v>0.2723995615</v>
       </c>
       <c r="D7">
-        <v>6.3306500000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>9.8166158000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>1.7985790630000002E-2</v>
+        <v>1.274157354E-2</v>
       </c>
       <c r="C8">
-        <v>0.1843929145</v>
+        <v>0.15343207010000001</v>
       </c>
       <c r="D8">
-        <v>6.2663700000000003E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.102880452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>3.1622998999999999E-2</v>
+        <v>2.2551621859999999E-2</v>
       </c>
       <c r="C9">
-        <v>0.20149679840000001</v>
+        <v>0.19250324560000001</v>
       </c>
       <c r="D9">
-        <v>6.25584E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.103446895</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>2.8738920179999999E-2</v>
+        <v>2.111328509E-2</v>
       </c>
       <c r="C10">
-        <v>0.21394323800000001</v>
+        <v>0.19735605449999999</v>
       </c>
       <c r="D10">
-        <v>6.2377799999999997E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.10368371699999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>2.1829531419999999E-2</v>
+        <v>2.5592825180000001E-2</v>
       </c>
       <c r="C11">
-        <v>0.2009338681</v>
+        <v>0.2119957194</v>
       </c>
       <c r="D11">
-        <v>6.2131800000000001E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.10358107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13">
-        <f>AVERAGE(B11)</f>
-        <v>2.1829531419999999E-2</v>
+        <f>AVERAGE(B2:B11)</f>
+        <v>4.7241828251999997E-2</v>
       </c>
       <c r="C13">
         <f>AVERAGE(C2:C11)</f>
-        <v>0.18480275751</v>
+        <v>0.21649908003000001</v>
       </c>
       <c r="D13">
         <f>AVERAGE(D2:D11)</f>
-        <v>6.3737769999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.1004671904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14">
         <f>_xlfn.STDEV.S(B2:B11)</f>
-        <v>6.0641477482463796E-3</v>
+        <v>5.9943214529267506E-2</v>
       </c>
       <c r="C14">
         <f>_xlfn.STDEV.S(C2:C11)</f>
-        <v>2.2758862922118494E-2</v>
+        <v>6.6044186394688079E-2</v>
       </c>
       <c r="D14">
         <f>_xlfn.STDEV.S(D2:D11)</f>
-        <v>2.6716434966972016E-3</v>
+        <v>1.1143934629020639E-2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Calculated average of variances instead of std's
</commit_message>
<xml_diff>
--- a/Project3/brute_data_6.xlsx
+++ b/Project3/brute_data_6.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tore/Documents/2019 høst/Computational-Physics-group/Project3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E9819B3-0E85-3E45-AF43-9D17DD8F9CD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2254FA-7ED1-5142-B980-891CFA5B248A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="500" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="brute_data_6" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>STD</t>
   </si>
@@ -43,11 +43,17 @@
   <si>
     <t>Avg</t>
   </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -881,137 +887,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>1.9327199999999999E-2</v>
       </c>
       <c r="C2">
+        <f>B2^2</f>
+        <v>3.7354065983999997E-4</v>
+      </c>
+      <c r="D2">
         <v>0.1962515702</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.113072359</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1.783849425E-2</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:C11" si="0">B3^2</f>
+        <v>3.1821187710728306E-4</v>
+      </c>
+      <c r="D3">
         <v>0.1821007526</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>9.8292862999999994E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1.276449707E-2</v>
       </c>
       <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1.629323854500386E-4</v>
+      </c>
+      <c r="D4">
         <v>0.14638135290000001</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>7.1126959000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>5.3309816060000001E-2</v>
       </c>
       <c r="C5">
+        <f t="shared" si="0"/>
+        <v>2.8419364883510339E-3</v>
+      </c>
+      <c r="D5">
         <v>0.24086790890000001</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.107232693</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>0.20664666340000001</v>
       </c>
       <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4.2702843494352903E-2</v>
+      </c>
+      <c r="D6">
         <v>0.37170256460000001</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.103188738</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>8.0532306070000004E-2</v>
       </c>
       <c r="C7">
+        <f t="shared" si="0"/>
+        <v>6.4854523209521599E-3</v>
+      </c>
+      <c r="D7">
         <v>0.2723995615</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>9.8166158000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>1.274157354E-2</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1.6234769627522814E-4</v>
+      </c>
+      <c r="D8">
         <v>0.15343207010000001</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.102880452</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>2.2551621859999999E-2</v>
       </c>
       <c r="C9">
+        <f t="shared" si="0"/>
+        <v>5.0857564851642984E-4</v>
+      </c>
+      <c r="D9">
         <v>0.19250324560000001</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.103446895</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>2.111328509E-2</v>
       </c>
       <c r="C10">
+        <f t="shared" si="0"/>
+        <v>4.4577080729161627E-4</v>
+      </c>
+      <c r="D10">
         <v>0.19735605449999999</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.10368371699999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>2.5592825180000001E-2</v>
       </c>
       <c r="C11">
+        <f t="shared" si="0"/>
+        <v>6.5499270069404203E-4</v>
+      </c>
+      <c r="D11">
         <v>0.2119957194</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.10358107</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1021,28 +1070,37 @@
       </c>
       <c r="C13">
         <f>AVERAGE(C2:C11)</f>
-        <v>0.21649908003000001</v>
+        <v>5.4656604078830735E-3</v>
       </c>
       <c r="D13">
         <f>AVERAGE(D2:D11)</f>
+        <v>0.21649908003000001</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(E2:E11)</f>
         <v>0.1004671904</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14">
-        <f>_xlfn.STDEV.S(B2:B11)</f>
-        <v>5.9943214529267506E-2</v>
-      </c>
-      <c r="C14">
-        <f>_xlfn.STDEV.S(C2:C11)</f>
-        <v>6.6044186394688079E-2</v>
-      </c>
       <c r="D14">
         <f>_xlfn.STDEV.S(D2:D11)</f>
+        <v>6.6044186394688079E-2</v>
+      </c>
+      <c r="E14">
+        <f>_xlfn.STDEV.S(E2:E11)</f>
         <v>1.1143934629020639E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <f>SQRT(C13)</f>
+        <v>7.3930104882132239E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>